<commit_message>
Finished Plate. Fixed errors (missing via, missing solder mask) on BlueMacro
</commit_message>
<xml_diff>
--- a/BlueMacro840/BlueMacro-top-pos.xlsx
+++ b/BlueMacro840/BlueMacro-top-pos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\NRF52-Board-master\BlueMacro840\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\crispy-keyboard-NRF52\BlueMacro840\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{246A1600-9526-4A9B-A5D7-A34BD4385003}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02E209E1-BE2E-4CB1-82B7-69135F373BDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="2160" yWindow="2160" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BlueMacro-top-pos" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="59">
   <si>
     <t>Designator</t>
   </si>
@@ -188,12 +188,21 @@
   </si>
   <si>
     <t>Crystal_SMD_3215-2Pin_3.2x1.5mm</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>E73-2G4M08S1C</t>
+  </si>
+  <si>
+    <t>E73-2G4M08S1C-52840</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1027,10 +1036,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1563,6 +1574,29 @@
         <v>10</v>
       </c>
     </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24" t="s">
+        <v>58</v>
+      </c>
+      <c r="D24">
+        <v>48260000</v>
+      </c>
+      <c r="E24">
+        <v>-56515000</v>
+      </c>
+      <c r="F24">
+        <v>270000000</v>
+      </c>
+      <c r="G24" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>